<commit_message>
Start breaking down Alt1
</commit_message>
<xml_diff>
--- a/CH-136 Column Splitting.xlsx
+++ b/CH-136 Column Splitting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616E6FCC-650A-4F6A-B636-345062DEF54E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136EFA08-E8C3-4A79-8524-7852112FC335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9355,7 +9355,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9674,6 +9674,10 @@
       <c r="F12" t="str">
         <v/>
       </c>
+      <c r="H12" t="str" cm="1">
+        <f t="array" ref="H12:H17">_xlfn.REGEXREPLACE(B3:B8,"(?=(.)).(?=\1)","$1,")</f>
+        <v>MXN,N1</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
@@ -9687,6 +9691,9 @@
       <c r="F13" t="str">
         <v>F12</v>
       </c>
+      <c r="H13" t="str">
+        <v>F,F,F12</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
@@ -9700,6 +9707,9 @@
       <c r="F14" t="str">
         <v/>
       </c>
+      <c r="H14" t="str">
+        <v>RSN</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="18"/>
@@ -9712,6 +9722,9 @@
       <c r="F15" t="str">
         <v/>
       </c>
+      <c r="H15" t="str">
+        <v>HN,NM</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="18"/>
@@ -9724,8 +9737,11 @@
       <c r="F16" t="str">
         <v/>
       </c>
-    </row>
-    <row r="17" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H16" t="str">
+        <v>RQ12,21</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="18"/>
       <c r="D17" s="17" t="str">
         <v>O2</v>
@@ -9736,64 +9752,67 @@
       <c r="F17" t="str">
         <v>O</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H17" t="str">
+        <v>O2,2O,O</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="18"/>
       <c r="D18" s="17"/>
     </row>
-    <row r="19" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="18"/>
       <c r="D19" s="17"/>
     </row>
-    <row r="20" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="18"/>
       <c r="D20" s="17"/>
     </row>
-    <row r="21" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="18"/>
       <c r="D21" s="17"/>
     </row>
-    <row r="22" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="18"/>
       <c r="D22" s="17"/>
     </row>
-    <row r="23" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="18"/>
       <c r="D23" s="17"/>
     </row>
-    <row r="24" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="18"/>
       <c r="D24" s="17"/>
     </row>
-    <row r="25" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="18"/>
       <c r="D25" s="17"/>
     </row>
-    <row r="26" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="18"/>
       <c r="D26" s="17"/>
     </row>
-    <row r="27" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="18"/>
       <c r="D27" s="17"/>
     </row>
-    <row r="28" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="18"/>
       <c r="D28" s="17"/>
     </row>
-    <row r="29" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="18"/>
       <c r="D29" s="17"/>
     </row>
-    <row r="30" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="18"/>
       <c r="D30" s="17"/>
     </row>
-    <row r="31" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="18"/>
       <c r="D31" s="17"/>
     </row>
-    <row r="32" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="18"/>
       <c r="D32" s="17"/>
     </row>

</xml_diff>

<commit_message>
Came up with alternative regex
</commit_message>
<xml_diff>
--- a/CH-136 Column Splitting.xlsx
+++ b/CH-136 Column Splitting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10D524A-379E-4CC5-9D54-B7F4C6304AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF43837-8F2E-4FCD-B3D7-743C98C633D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="25">
   <si>
     <t>Question</t>
   </si>
@@ -136,6 +136,9 @@
   <si>
     <t>RegEx</t>
   </si>
+  <si>
+    <t>This is a simpler lookahead</t>
+  </si>
 </sst>
 </file>
 
@@ -144,7 +147,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,6 +190,13 @@
       <color theme="1"/>
       <name val="Century Gothic"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -357,10 +367,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -413,7 +423,8 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Intro_Hd" xfId="2" xr:uid="{10F89C6A-8E93-4B98-BD22-C0C241F41FF3}"/>
@@ -5077,8 +5088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4055AD7-3F97-4A30-9277-C2FB6C75AFA9}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5512,67 +5523,122 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="18"/>
       <c r="D17" s="17"/>
     </row>
-    <row r="18" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="18"/>
-      <c r="D18" s="17"/>
-    </row>
-    <row r="19" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="17" t="str" cm="1">
+        <f t="array" ref="D18:F23">_xlfn.LET(
+_xlpm.d, _xlfn.REGEXREPLACE(B3:B8,"(.)(?=\1)","$1,"),
+_xlfn.DROP(_xlfn.IFNA(_xlfn.REDUCE("",_xlpm.d,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.TEXTSPLIT(_xlpm.v,",")))),""),1)
+)</f>
+        <v>MXN</v>
+      </c>
+      <c r="E18" t="str">
+        <v>N1</v>
+      </c>
+      <c r="F18" t="str">
+        <v/>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="18"/>
-      <c r="D19" s="17"/>
-    </row>
-    <row r="20" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="17" t="str">
+        <v>F</v>
+      </c>
+      <c r="E19" t="str">
+        <v>F</v>
+      </c>
+      <c r="F19" t="str">
+        <v>F12</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="18"/>
-      <c r="D20" s="17"/>
-    </row>
-    <row r="21" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="17" t="str">
+        <v>RSN</v>
+      </c>
+      <c r="E20" t="str">
+        <v/>
+      </c>
+      <c r="F20" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="18"/>
-      <c r="D21" s="17"/>
-    </row>
-    <row r="22" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="17" t="str">
+        <v>HN</v>
+      </c>
+      <c r="E21" t="str">
+        <v>NM</v>
+      </c>
+      <c r="F21" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="18"/>
-      <c r="D22" s="17"/>
-    </row>
-    <row r="23" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="17" t="str">
+        <v>RQ12</v>
+      </c>
+      <c r="E22" t="str">
+        <v>21</v>
+      </c>
+      <c r="F22" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="18"/>
-      <c r="D23" s="17"/>
-    </row>
-    <row r="24" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="17" t="str">
+        <v>O2</v>
+      </c>
+      <c r="E23" t="str">
+        <v>2O</v>
+      </c>
+      <c r="F23" t="str">
+        <v>O</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="18"/>
       <c r="D24" s="17"/>
     </row>
-    <row r="25" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="18"/>
       <c r="D25" s="17"/>
     </row>
-    <row r="26" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="18"/>
       <c r="D26" s="17"/>
     </row>
-    <row r="27" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="18"/>
       <c r="D27" s="17"/>
     </row>
-    <row r="28" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="18"/>
       <c r="D28" s="17"/>
     </row>
-    <row r="29" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="18"/>
       <c r="D29" s="17"/>
     </row>
-    <row r="30" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="18"/>
       <c r="D30" s="17"/>
     </row>
-    <row r="31" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="18"/>
       <c r="D31" s="17"/>
     </row>
-    <row r="32" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="18"/>
       <c r="D32" s="17"/>
     </row>

</xml_diff>

<commit_message>
Look at more regex options
</commit_message>
<xml_diff>
--- a/CH-136 Column Splitting.xlsx
+++ b/CH-136 Column Splitting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF43837-8F2E-4FCD-B3D7-743C98C633D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{873B0E67-1240-4172-963E-0AFF426859AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="27">
   <si>
     <t>Question</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>This is a simpler lookahead</t>
+  </si>
+  <si>
+    <t>Good regex reference</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/2126137/regex-lookahead-ordering</t>
   </si>
 </sst>
 </file>
@@ -5088,8 +5094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4055AD7-3F97-4A30-9277-C2FB6C75AFA9}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5224,9 +5230,13 @@
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
+      <c r="I4" s="11" t="s">
+        <v>25</v>
+      </c>
       <c r="J4" s="11"/>
-      <c r="K4" s="7"/>
+      <c r="K4" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>

</xml_diff>